<commit_message>
* add template example * function to add a template to settings * function to copy templates excel file
</commit_message>
<xml_diff>
--- a/src/vlinder_toolkit/data_templates/csv_templates.xlsx
+++ b/src/vlinder_toolkit/data_templates/csv_templates.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="vlinder_template" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="mocca_template" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="vlinder_metadata_template" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="67">
   <si>
     <t xml:space="preserve">varname</t>
   </si>
@@ -189,6 +190,39 @@
   </si>
   <si>
     <t xml:space="preserve">active 2m-temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLINDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">call_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">benaming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network</t>
   </si>
 </sst>
 </file>
@@ -403,17 +437,17 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.25"/>
   </cols>
@@ -712,11 +746,11 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26"/>
@@ -936,4 +970,218 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add template for general datafiles (Amber)
</commit_message>
<xml_diff>
--- a/src/vlinder_toolkit/data_templates/csv_templates.xlsx
+++ b/src/vlinder_toolkit/data_templates/csv_templates.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vlinder_template" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="mocca_template" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="vlinder_metadata_template" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="basic_amber_format" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
   <si>
     <t xml:space="preserve">varname</t>
   </si>
@@ -223,6 +224,15 @@
   </si>
   <si>
     <t xml:space="preserve">Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
   </si>
 </sst>
 </file>
@@ -438,14 +448,14 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.12"/>
@@ -750,7 +760,7 @@
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26"/>
@@ -979,8 +989,222 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1007,10 +1231,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1020,160 +1244,74 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>60</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Data templats from excel (#33)
* trigger action

* use small datasets for action test + fix the no coordinates

* fix missing lat lon in tests and adding meta data

* * csv templates are now read out of excel file.
* removed the default template settings --> extra check for template-uniqueness is implemented

* * add template example
* function to add a template to settings
* function to copy templates excel file

* Update master_test.yml

* deployed

* Update python_testing.yml

no /desktop in action

* fix possibilit if datetime column is present in dataset

* add template for general datafiles (Amber)

* _
</commit_message>
<xml_diff>
--- a/src/vlinder_toolkit/data_templates/csv_templates.xlsx
+++ b/src/vlinder_toolkit/data_templates/csv_templates.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vlinder_template" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="mocca_template" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="vlinder_metadata_template" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="basic_amber_format" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
   <si>
     <t xml:space="preserve">varname</t>
   </si>
@@ -223,6 +224,15 @@
   </si>
   <si>
     <t xml:space="preserve">Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
   </si>
 </sst>
 </file>
@@ -438,14 +448,14 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.12"/>
@@ -750,7 +760,7 @@
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26"/>
@@ -979,8 +989,222 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1007,10 +1231,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1020,160 +1244,74 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>60</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Restored files and add solution for issues 43 and 44.
</commit_message>
<xml_diff>
--- a/src/vlinder_toolkit/data_templates/csv_templates.xlsx
+++ b/src/vlinder_toolkit/data_templates/csv_templates.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="71">
   <si>
     <t xml:space="preserve">varname</t>
   </si>
@@ -229,10 +229,13 @@
     <t xml:space="preserve">station</t>
   </si>
   <si>
-    <t xml:space="preserve">DateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value</t>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flags</t>
   </si>
 </sst>
 </file>
@@ -455,7 +458,7 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.12"/>
@@ -760,7 +763,7 @@
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26"/>
@@ -993,7 +996,7 @@
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1201,13 +1204,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1252,40 +1255,44 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
@@ -1300,7 +1307,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>19</v>
@@ -1312,6 +1319,26 @@
         <v>21</v>
       </c>
       <c r="F8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fix pie charts when 1 station selected
</commit_message>
<xml_diff>
--- a/src/vlinder_toolkit/data_templates/csv_templates.xlsx
+++ b/src/vlinder_toolkit/data_templates/csv_templates.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="74">
   <si>
     <t xml:space="preserve">varname</t>
   </si>
@@ -236,6 +236,15 @@
   </si>
   <si>
     <t xml:space="preserve">flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%Y-%m-%dT%H:%M:%S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMP</t>
   </si>
 </sst>
 </file>
@@ -458,7 +467,7 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.12"/>
@@ -763,7 +772,7 @@
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26"/>
@@ -996,7 +1005,7 @@
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1204,13 +1213,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1335,10 +1344,53 @@
       <c r="A10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>